<commit_message>
Correção da conversão de float na função extract_google_finance e criação do readme.
</commit_message>
<xml_diff>
--- a/data/raw/Maiores Altas.xlsx
+++ b/data/raw/Maiores Altas.xlsx
@@ -476,7 +476,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>+6.89%</t>
+          <t>+6,89%</t>
         </is>
       </c>
       <c r="E2" t="n">
@@ -499,7 +499,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>+0.18%</t>
+          <t>+0,18%</t>
         </is>
       </c>
       <c r="E3" t="n">
@@ -522,7 +522,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>-0.15%</t>
+          <t>-0,15%</t>
         </is>
       </c>
       <c r="E4" t="n">
@@ -545,7 +545,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>+0.70%</t>
+          <t>+0,70%</t>
         </is>
       </c>
       <c r="E5" t="n">
@@ -568,7 +568,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>+1.15%</t>
+          <t>+1,15%</t>
         </is>
       </c>
       <c r="E6" t="n">

</xml_diff>